<commit_message>
entrar a segunda hoja de excel
</commit_message>
<xml_diff>
--- a/Documentos/HorariosCompletos.xlsx
+++ b/Documentos/HorariosCompletos.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAF8DD02-2054-4643-B414-2D5C9679DAC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9ED4FCC-6468-4864-BF29-8DF64E8588B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$N$477</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5748" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5751" uniqueCount="240">
   <si>
     <t>materia</t>
   </si>
@@ -707,13 +707,61 @@
   </si>
   <si>
     <t>B-25</t>
+  </si>
+  <si>
+    <t>Carrera</t>
+  </si>
+  <si>
+    <t>Cupo</t>
+  </si>
+  <si>
+    <t>INGENIERÍA AGROINDUSTRIAL</t>
+  </si>
+  <si>
+    <t>INGENIERÍA AMBIENTAL</t>
+  </si>
+  <si>
+    <t>INGENIERÍA EN GEOLOGÍA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA CIVIL</t>
+  </si>
+  <si>
+    <t>INGENIERÍA EN GEOINFORMÁTICA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA EN TOPOGRAFÍA Y CONSTRUCCIÓN</t>
+  </si>
+  <si>
+    <t>INGENIERÍA EN COMPUTACIÓN</t>
+  </si>
+  <si>
+    <t>INGENIERÍA EN SISTEMAS INTELIGENTES</t>
+  </si>
+  <si>
+    <t>INGENIERÍA EN ELECTRICIDAD Y AUTOMATIZACIÓN</t>
+  </si>
+  <si>
+    <t>INGENIERÍA EN MECATRÓNICA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA MECÁNICA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA MECÁNICA ADMINISTRATIVA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA MECÁNICA ELÉCTRICA</t>
+  </si>
+  <si>
+    <t>INGENIERÍA METALÚRGICA Y DE MATERIALES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -740,8 +788,19 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -752,6 +811,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF222A35"/>
         <bgColor rgb="FF222A35"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF222B35"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -774,7 +851,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -792,6 +869,23 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1010,7 +1104,7 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A475" sqref="A475"/>
+      <selection activeCell="L480" sqref="L480"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -22843,10 +22937,157 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="D1:E18"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="4" max="4" width="37.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:5">
+      <c r="D1" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="4:5">
+      <c r="D2" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="E2" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="4:5">
+      <c r="D3" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="E3" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5">
+      <c r="D4" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="E4" s="11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5">
+      <c r="D5" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="E5" s="11">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5">
+      <c r="D6" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" s="11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5">
+      <c r="D7" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="E7" s="11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5">
+      <c r="D8" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5">
+      <c r="D9" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="E9" s="11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5">
+      <c r="D10" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="E10" s="11">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5">
+      <c r="D11" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="E11" s="11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5">
+      <c r="D12" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E12" s="11">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5">
+      <c r="D13" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="E13" s="11">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5">
+      <c r="D14" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E14" s="11">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="4:5">
+      <c r="D15" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="E15" s="11">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="4:5" ht="15">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="4:4" ht="15">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="4:4" ht="15">
+      <c r="D18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F36453F-F3F4-434B-9A57-5F5DED3F96E6}">
   <dimension ref="B2:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D6" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -22903,84 +23144,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="D6:D18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
-  <sheetData>
-    <row r="6" spans="4:4" ht="15">
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="4:4" ht="15">
-      <c r="D7" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="4:4" ht="15">
-      <c r="D8" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="4:4" ht="15">
-      <c r="D9" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="4:4" ht="15">
-      <c r="D10" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="4:4" ht="15">
-      <c r="D11" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="12" spans="4:4" ht="15">
-      <c r="D12" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="4:4" ht="15">
-      <c r="D13" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="4:4" ht="15">
-      <c r="D14" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="15" spans="4:4" ht="15">
-      <c r="D15" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="16" spans="4:4" ht="15">
-      <c r="D16" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" ht="15">
-      <c r="D17" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" ht="15">
-      <c r="D18" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>